<commit_message>
Ver 0.0.0002   BehaviorTree for AI, uncomplete..
</commit_message>
<xml_diff>
--- a/数值表.xlsx
+++ b/数值表.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12240" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12240" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Roles" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="Buff" sheetId="1" r:id="rId5"/>
     <sheet name="Effect" sheetId="6" r:id="rId6"/>
     <sheet name="Relation" sheetId="5" r:id="rId7"/>
+    <sheet name="决策" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="358">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -701,6 +703,742 @@
   </si>
   <si>
     <t>material</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>进攻</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>防守</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>闲置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AI开启</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>模式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>挨打还手</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>进攻</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>某人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无视其他单位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消灭范围内其他单位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>某位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>警戒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>程度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>低</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>范围</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>移动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>死亡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>朝向/目标</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>濒死</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>溃散/激励</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>防御</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>朝向/目标</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>躲避</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>远离/闪避动作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>动作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>动作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>目标</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>相关性</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>躺了吧</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发呆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>懵在原地</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无cd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机选择释放</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有cd(长)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>准备就绪后释放</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无技能时</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>超出防守范围</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>具有一定的逻辑关系</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>血量少于危险血线</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>没血了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>府兵</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>散兵</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从据点生成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>队列整齐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>散落在野外</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三五成群</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>目标明确</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自主性较强</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无溃逃动作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>会溃逃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消灭防守区域的所有其他目标</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>会逃跑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>selector</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sequence</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>condition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>action</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>叶子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>执行第一个子节点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>顺序执行子节点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>打</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>防</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>躲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>呆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>溃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>亡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>共享情报</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>闲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>活着吗?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>亡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>残血吗?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发现敌人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>追</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有目标位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1/2骰子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>巡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>呆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有固有位置,有追击范围</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无固有位置.追到天荒地老</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>兵种</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>盾</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>戈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>弓</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>弩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>骑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>弓骑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>刀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>兵源属性</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小队编制</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>盾牌兵</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>刀斧手</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>矛兵</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>弓兵</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>弩兵</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>骑兵</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>车</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>战车</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>床</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>床弩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>弓骑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>移速</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击频率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击范围</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>低</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>近</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>远</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>远+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>低</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>低-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>低+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>远++</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>远-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>远+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>低</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击力度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高++</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>弹幕爆射</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多重射击</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>剑刃风暴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冲锋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蜂刺</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>盾牌冲锋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大风车</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>正前方爆刺</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前方扇形弹幕数轮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前方锥形弹幕爆射</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>连珠</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>朝目标的极速一串弹幕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>超出防守范围?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>平砍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向着目标放技能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>暂时不考虑自身增益问题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sequence</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>盾牌格挡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>挥砍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二连斩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>横扫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>平射</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>平射</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>间隔长于弓</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>策马冲锋, 大额伤害, 击飞</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>斩击</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自上而下的攻击</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>buff技能,大幅度提高防御力,大幅度降低移动速度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>举盾牌正前方冲刺, 正面无伤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能冷却?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击范围?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/远离了队长位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -733,12 +1471,42 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="16">
@@ -927,7 +1695,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1021,6 +1789,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1030,7 +1825,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1317,7 +2112,7 @@
   <dimension ref="A1:P52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:N28"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1710,8 +2505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2164,7 +2959,7 @@
   <dimension ref="B3:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="E6" sqref="E6:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2185,16 +2980,16 @@
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" s="25"/>
       <c r="D4" s="14"/>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31" t="s">
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" s="16" t="s">
@@ -2608,7 +3403,7 @@
       <c r="J34" s="14"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B35" s="34">
+      <c r="B35" s="31">
         <v>30</v>
       </c>
       <c r="D35" s="14"/>
@@ -2633,8 +3428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2647,16 +3442,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31" t="s">
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B3" s="15" t="s">
@@ -2883,7 +3678,7 @@
   <dimension ref="B2:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34:K34"/>
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2905,18 +3700,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="F2" s="33"/>
-      <c r="G2" s="32" t="s">
+      <c r="F2" s="42"/>
+      <c r="G2" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="H2" s="33"/>
-      <c r="I2" s="32" t="s">
+      <c r="H2" s="42"/>
+      <c r="I2" s="41" t="s">
         <v>126</v>
       </c>
-      <c r="J2" s="33"/>
+      <c r="J2" s="42"/>
       <c r="K2" s="14" t="s">
         <v>164</v>
       </c>
@@ -3739,7 +4534,7 @@
   <dimension ref="A3:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3814,4 +4609,856 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G4" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.125" customWidth="1"/>
+    <col min="9" max="9" width="11.75" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.375" customWidth="1"/>
+    <col min="12" max="12" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.25" customWidth="1"/>
+    <col min="14" max="14" width="13.75" customWidth="1"/>
+    <col min="15" max="15" width="11.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>238</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>239</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>244</v>
+      </c>
+      <c r="I4" t="s">
+        <v>255</v>
+      </c>
+      <c r="J4" s="32" t="s">
+        <v>239</v>
+      </c>
+      <c r="K4" s="33" t="s">
+        <v>240</v>
+      </c>
+      <c r="L4" s="34" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F5" s="33" t="s">
+        <v>240</v>
+      </c>
+      <c r="G5" s="33" t="s">
+        <v>245</v>
+      </c>
+      <c r="L5" s="35" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F6" s="34" t="s">
+        <v>241</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>243</v>
+      </c>
+      <c r="K6" s="33" t="s">
+        <v>240</v>
+      </c>
+      <c r="L6" s="34" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B7" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>242</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>243</v>
+      </c>
+      <c r="L7" s="35" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D8" t="s">
+        <v>186</v>
+      </c>
+      <c r="K8" s="33" t="s">
+        <v>240</v>
+      </c>
+      <c r="L8" s="34" t="s">
+        <v>332</v>
+      </c>
+      <c r="M8" s="34" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C9" t="s">
+        <v>184</v>
+      </c>
+      <c r="D9" t="s">
+        <v>187</v>
+      </c>
+      <c r="L9" s="35" t="s">
+        <v>246</v>
+      </c>
+      <c r="M9" s="35" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>182</v>
+      </c>
+      <c r="C10" t="s">
+        <v>185</v>
+      </c>
+      <c r="D10" t="s">
+        <v>186</v>
+      </c>
+      <c r="K10" s="33" t="s">
+        <v>240</v>
+      </c>
+      <c r="L10" s="34" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>176</v>
+      </c>
+      <c r="C11" t="s">
+        <v>185</v>
+      </c>
+      <c r="D11" t="s">
+        <v>187</v>
+      </c>
+      <c r="L11" s="32" t="s">
+        <v>239</v>
+      </c>
+      <c r="M11" s="33" t="s">
+        <v>338</v>
+      </c>
+      <c r="N11" s="34" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N12" s="34" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>177</v>
+      </c>
+      <c r="C13" t="s">
+        <v>188</v>
+      </c>
+      <c r="D13" t="s">
+        <v>237</v>
+      </c>
+      <c r="N13" s="32" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M14" s="35" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K15" s="33" t="s">
+        <v>240</v>
+      </c>
+      <c r="L15" s="34" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B16" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="L16" s="35" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>253</v>
+      </c>
+      <c r="B17" t="s">
+        <v>197</v>
+      </c>
+      <c r="C17" t="s">
+        <v>200</v>
+      </c>
+      <c r="K17" s="33" t="s">
+        <v>240</v>
+      </c>
+      <c r="L17" s="34" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>246</v>
+      </c>
+      <c r="B18" t="s">
+        <v>221</v>
+      </c>
+      <c r="C18" t="s">
+        <v>222</v>
+      </c>
+      <c r="E18" t="s">
+        <v>223</v>
+      </c>
+      <c r="L18" s="35" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="38" t="s">
+        <v>247</v>
+      </c>
+      <c r="B19" s="38" t="s">
+        <v>196</v>
+      </c>
+      <c r="C19" s="38" t="s">
+        <v>199</v>
+      </c>
+      <c r="D19" s="38" t="s">
+        <v>335</v>
+      </c>
+      <c r="E19" s="43" t="s">
+        <v>224</v>
+      </c>
+      <c r="K19" s="35" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="39" t="s">
+        <v>248</v>
+      </c>
+      <c r="B20" s="39" t="s">
+        <v>203</v>
+      </c>
+      <c r="C20" s="39" t="s">
+        <v>204</v>
+      </c>
+      <c r="D20" s="39"/>
+      <c r="E20" s="43"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="39" t="s">
+        <v>249</v>
+      </c>
+      <c r="B21" s="39" t="s">
+        <v>205</v>
+      </c>
+      <c r="C21" s="39" t="s">
+        <v>206</v>
+      </c>
+      <c r="D21" s="39"/>
+      <c r="E21" s="43"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="38" t="s">
+        <v>250</v>
+      </c>
+      <c r="B22" s="38" t="s">
+        <v>212</v>
+      </c>
+      <c r="C22" s="38" t="s">
+        <v>213</v>
+      </c>
+      <c r="D22" s="38"/>
+      <c r="E22" s="43"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="38" t="s">
+        <v>333</v>
+      </c>
+      <c r="B23" s="38" t="s">
+        <v>334</v>
+      </c>
+      <c r="C23" s="38" t="s">
+        <v>336</v>
+      </c>
+      <c r="D23" s="38" t="s">
+        <v>337</v>
+      </c>
+      <c r="E23" s="43"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>251</v>
+      </c>
+      <c r="B24" t="s">
+        <v>201</v>
+      </c>
+      <c r="C24" t="s">
+        <v>202</v>
+      </c>
+      <c r="E24" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>252</v>
+      </c>
+      <c r="B25" t="s">
+        <v>198</v>
+      </c>
+      <c r="C25" t="s">
+        <v>211</v>
+      </c>
+      <c r="E25" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>215</v>
+      </c>
+      <c r="C27" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>217</v>
+      </c>
+      <c r="C28" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>219</v>
+      </c>
+      <c r="C29" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>189</v>
+      </c>
+      <c r="C32" t="s">
+        <v>190</v>
+      </c>
+      <c r="D32" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>192</v>
+      </c>
+      <c r="D35" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>275</v>
+      </c>
+      <c r="C39" t="s">
+        <v>227</v>
+      </c>
+      <c r="D39" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
+        <v>229</v>
+      </c>
+      <c r="D40" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
+        <v>230</v>
+      </c>
+      <c r="D41" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C42" t="s">
+        <v>233</v>
+      </c>
+      <c r="D42" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
+        <v>235</v>
+      </c>
+      <c r="D43" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C44" t="s">
+        <v>265</v>
+      </c>
+      <c r="D44" t="s">
+        <v>266</v>
+      </c>
+      <c r="H44" t="s">
+        <v>267</v>
+      </c>
+      <c r="I44" t="s">
+        <v>289</v>
+      </c>
+      <c r="J44" t="s">
+        <v>314</v>
+      </c>
+      <c r="K44" t="s">
+        <v>291</v>
+      </c>
+      <c r="L44" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="F45" s="36"/>
+      <c r="G45" t="s">
+        <v>268</v>
+      </c>
+      <c r="H45" t="s">
+        <v>277</v>
+      </c>
+      <c r="I45" t="s">
+        <v>292</v>
+      </c>
+      <c r="J45" t="s">
+        <v>302</v>
+      </c>
+      <c r="K45" t="s">
+        <v>294</v>
+      </c>
+      <c r="L45" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="F46" s="36"/>
+      <c r="G46" t="s">
+        <v>274</v>
+      </c>
+      <c r="H46" t="s">
+        <v>278</v>
+      </c>
+      <c r="I46" t="s">
+        <v>306</v>
+      </c>
+      <c r="J46" t="s">
+        <v>296</v>
+      </c>
+      <c r="K46" t="s">
+        <v>294</v>
+      </c>
+      <c r="L46" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>276</v>
+      </c>
+      <c r="F47" s="36"/>
+      <c r="G47" t="s">
+        <v>269</v>
+      </c>
+      <c r="H47" t="s">
+        <v>279</v>
+      </c>
+      <c r="I47" t="s">
+        <v>300</v>
+      </c>
+      <c r="J47" t="s">
+        <v>317</v>
+      </c>
+      <c r="K47" t="s">
+        <v>297</v>
+      </c>
+      <c r="L47" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>254</v>
+      </c>
+      <c r="F48" s="36"/>
+      <c r="G48" t="s">
+        <v>270</v>
+      </c>
+      <c r="H48" t="s">
+        <v>280</v>
+      </c>
+      <c r="I48" t="s">
+        <v>300</v>
+      </c>
+      <c r="J48" t="s">
+        <v>296</v>
+      </c>
+      <c r="K48" t="s">
+        <v>298</v>
+      </c>
+      <c r="L48" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="49" spans="6:14" x14ac:dyDescent="0.2">
+      <c r="F49" s="36"/>
+      <c r="G49" t="s">
+        <v>271</v>
+      </c>
+      <c r="H49" t="s">
+        <v>281</v>
+      </c>
+      <c r="I49" t="s">
+        <v>305</v>
+      </c>
+      <c r="J49" t="s">
+        <v>288</v>
+      </c>
+      <c r="K49" t="s">
+        <v>299</v>
+      </c>
+      <c r="L49" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="50" spans="6:14" x14ac:dyDescent="0.2">
+      <c r="F50" s="36"/>
+      <c r="G50" t="s">
+        <v>272</v>
+      </c>
+      <c r="H50" t="s">
+        <v>282</v>
+      </c>
+      <c r="I50" t="s">
+        <v>288</v>
+      </c>
+      <c r="J50" t="s">
+        <v>301</v>
+      </c>
+      <c r="K50" t="s">
+        <v>297</v>
+      </c>
+      <c r="L50" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="51" spans="6:14" x14ac:dyDescent="0.2">
+      <c r="F51" s="36"/>
+      <c r="G51" t="s">
+        <v>273</v>
+      </c>
+      <c r="H51" t="s">
+        <v>287</v>
+      </c>
+      <c r="I51" t="s">
+        <v>301</v>
+      </c>
+      <c r="J51" t="s">
+        <v>295</v>
+      </c>
+      <c r="K51" t="s">
+        <v>308</v>
+      </c>
+      <c r="L51" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="52" spans="6:14" x14ac:dyDescent="0.2">
+      <c r="F52" s="36"/>
+      <c r="G52" t="s">
+        <v>283</v>
+      </c>
+      <c r="H52" t="s">
+        <v>284</v>
+      </c>
+      <c r="I52" t="s">
+        <v>303</v>
+      </c>
+      <c r="J52" t="s">
+        <v>316</v>
+      </c>
+      <c r="K52" t="s">
+        <v>309</v>
+      </c>
+      <c r="L52" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="53" spans="6:14" x14ac:dyDescent="0.2">
+      <c r="F53" s="36"/>
+      <c r="G53" t="s">
+        <v>285</v>
+      </c>
+      <c r="H53" t="s">
+        <v>286</v>
+      </c>
+      <c r="I53" t="s">
+        <v>304</v>
+      </c>
+      <c r="J53" t="s">
+        <v>315</v>
+      </c>
+      <c r="K53" t="s">
+        <v>307</v>
+      </c>
+      <c r="L53" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="62" spans="6:14" x14ac:dyDescent="0.2">
+      <c r="H62" t="s">
+        <v>318</v>
+      </c>
+      <c r="J62" t="s">
+        <v>319</v>
+      </c>
+      <c r="L62" t="s">
+        <v>341</v>
+      </c>
+      <c r="N62" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="63" spans="6:14" ht="57" x14ac:dyDescent="0.2">
+      <c r="G63" t="s">
+        <v>268</v>
+      </c>
+      <c r="H63" t="s">
+        <v>340</v>
+      </c>
+      <c r="I63" s="37" t="s">
+        <v>352</v>
+      </c>
+      <c r="J63" t="s">
+        <v>343</v>
+      </c>
+      <c r="L63" t="s">
+        <v>325</v>
+      </c>
+      <c r="M63" s="37" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="64" spans="6:14" x14ac:dyDescent="0.2">
+      <c r="G64" t="s">
+        <v>274</v>
+      </c>
+      <c r="H64" t="s">
+        <v>344</v>
+      </c>
+      <c r="I64" s="37"/>
+      <c r="L64" t="s">
+        <v>322</v>
+      </c>
+      <c r="M64" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="65" spans="7:13" x14ac:dyDescent="0.2">
+      <c r="G65" t="s">
+        <v>269</v>
+      </c>
+      <c r="H65" t="s">
+        <v>345</v>
+      </c>
+      <c r="I65" s="37"/>
+      <c r="L65" t="s">
+        <v>324</v>
+      </c>
+      <c r="M65" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="66" spans="7:13" x14ac:dyDescent="0.2">
+      <c r="G66" t="s">
+        <v>270</v>
+      </c>
+      <c r="H66" t="s">
+        <v>346</v>
+      </c>
+      <c r="I66" s="37"/>
+      <c r="L66" t="s">
+        <v>321</v>
+      </c>
+      <c r="M66" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="67" spans="7:13" x14ac:dyDescent="0.2">
+      <c r="G67" t="s">
+        <v>271</v>
+      </c>
+      <c r="H67" t="s">
+        <v>347</v>
+      </c>
+      <c r="I67" s="37" t="s">
+        <v>348</v>
+      </c>
+      <c r="L67" t="s">
+        <v>320</v>
+      </c>
+      <c r="M67" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="68" spans="7:13" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="G68" t="s">
+        <v>272</v>
+      </c>
+      <c r="H68" t="s">
+        <v>350</v>
+      </c>
+      <c r="I68" s="37" t="s">
+        <v>351</v>
+      </c>
+      <c r="L68" t="s">
+        <v>323</v>
+      </c>
+      <c r="M68" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="69" spans="7:13" x14ac:dyDescent="0.2">
+      <c r="G69" t="s">
+        <v>273</v>
+      </c>
+      <c r="I69" s="37"/>
+      <c r="L69" t="s">
+        <v>330</v>
+      </c>
+      <c r="M69" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="70" spans="7:13" x14ac:dyDescent="0.2">
+      <c r="G70" t="s">
+        <v>283</v>
+      </c>
+      <c r="I70" s="37"/>
+    </row>
+    <row r="71" spans="7:13" x14ac:dyDescent="0.2">
+      <c r="G71" t="s">
+        <v>285</v>
+      </c>
+      <c r="I71" s="37"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E19:E23"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ver 0.0.0003   todo: evaluators & actions
</commit_message>
<xml_diff>
--- a/数值表.xlsx
+++ b/数值表.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="399">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -906,10 +906,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>具有一定的逻辑关系</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>血量少于危险血线</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1030,10 +1026,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>闲</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>活着吗?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1050,395 +1042,567 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>有目标位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>呆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有固有位置,有追击范围</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无固有位置.追到天荒地老</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>兵种</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>盾</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>戈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>弓</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>弩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>骑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>弓骑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>刀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>兵源属性</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小队编制</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>盾牌兵</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>刀斧手</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>矛兵</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>弓兵</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>弩兵</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>骑兵</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>车</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>战车</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>床</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>床弩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>弓骑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>移速</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击频率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击范围</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>低</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>近</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>远</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>远+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>低</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>低-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>低+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>远++</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>远-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>远+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>低</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击力度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高++</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>弹幕爆射</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多重射击</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>剑刃风暴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冲锋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蜂刺</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>盾牌冲锋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大风车</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>正前方爆刺</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前方扇形弹幕数轮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前方锥形弹幕爆射</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>连珠</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>朝目标的极速一串弹幕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>超出防守范围?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>平砍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向着目标放技能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>盾牌格挡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>挥砍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二连斩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>横扫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>平射</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>平射</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>间隔长于弓</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>策马冲锋, 大额伤害, 击飞</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>斩击</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自上而下的攻击</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>buff技能,大幅度提高防御力,大幅度降低移动速度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>举盾牌正前方冲刺, 正面无伤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击范围?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/远离了队长位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>溃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sequence</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sequence</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>selector</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>全假才返回假</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>遇假则返回假</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>砍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能范围?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击范围?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>闪躲意向骰子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>周围无敌人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>到达队长附近</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>动作结束</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>动作结束</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能1准备?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能2准备?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直到</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>没了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>按照CD, 从高到低放</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卡cd放</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>距离过近?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>迅速闪身, 直到离开目标多少步</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>呆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>歇息若干秒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>追</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>有目标位置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1/2骰子</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>巡</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>呆</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有固有位置,有追击范围</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>无固有位置.追到天荒地老</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>兵种</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>盾</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>戈</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>弓</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>弩</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>骑</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>弓骑</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>刀</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>兵源属性</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>小队编制</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>盾牌兵</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>刀斧手</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>矛兵</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>弓兵</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>弩兵</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>骑兵</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>车</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>战车</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>床</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>床弩</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>弓骑</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>高</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>移速</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>攻击频率</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>攻击范围</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>中</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>低</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>近</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>中</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>中</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>中</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>远</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>远+</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>中-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>高</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>低</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>中+</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>低-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>低+</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>中+</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>远++</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>远-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>远+</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>低</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>高</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>中</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>中</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>攻击力度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>高++</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>高+</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>高</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>技1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>技2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>弹幕爆射</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>多重射击</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>剑刃风暴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>冲锋</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>蜂刺</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>盾牌冲锋</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>大风车</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>正前方爆刺</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>前方扇形弹幕数轮</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>前方锥形弹幕爆射</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>连珠</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>朝目标的极速一串弹幕</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>超出防守范围?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>技</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>技能</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>平砍</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>向着目标放技能</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>暂时不考虑自身增益问题</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sequence</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>技</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>盾牌格挡</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>技3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>技4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>挥砍</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>二连斩</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>横扫</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>平射</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>平射</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>间隔长于弓</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>策马冲锋, 大额伤害, 击飞</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>斩击</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>自上而下的攻击</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>buff技能,大幅度提高防御力,大幅度降低移动速度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>举盾牌正前方冲刺, 正面无伤</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>技能冷却?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>攻击范围?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/远离了队长位置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>返</t>
+    <t>远离了队长位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsAlive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HasCriticalHealth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OutOfGuardRange</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FarAwayFromCaptain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HasEnemy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WithinSkillRange</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WithinSlashRange</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DodgeDice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HasPositon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TooClose</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在sequ中直接跳过</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始/循环/终止</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>闲置模式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击模式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>躲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>闪躲意向骰子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>相当于if...else…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>parelle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>random</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>全部执行, 并根据所有返回结果返回</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机返回一个子节点</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1471,7 +1635,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1505,6 +1669,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1695,7 +1865,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1828,6 +1998,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="百分比" xfId="1" builtinId="5"/>
@@ -1844,6 +2020,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>761630</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>47558</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="图片 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{540CD22C-71B5-4820-9D15-321FACB62013}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7239000" y="3133725"/>
+          <a:ext cx="2961905" cy="533333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4613,10 +4838,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N71"/>
+  <dimension ref="A1:T71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G4" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4626,7 +4851,7 @@
     <col min="5" max="5" width="19.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.125" customWidth="1"/>
+    <col min="8" max="8" width="17.375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.75" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.375" customWidth="1"/>
@@ -4634,19 +4859,22 @@
     <col min="13" max="13" width="17.25" customWidth="1"/>
     <col min="14" max="14" width="13.75" customWidth="1"/>
     <col min="15" max="15" width="11.875" customWidth="1"/>
+    <col min="16" max="16" width="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>178</v>
       </c>
@@ -4654,55 +4882,82 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
+        <v>237</v>
+      </c>
+      <c r="F4" s="32" t="s">
         <v>238</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="G4" s="32" t="s">
+        <v>243</v>
+      </c>
+      <c r="H4" t="s">
+        <v>353</v>
+      </c>
+      <c r="I4" s="45" t="s">
+        <v>390</v>
+      </c>
+      <c r="J4" s="32" t="s">
+        <v>352</v>
+      </c>
+      <c r="K4" s="33" t="s">
         <v>239</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="L4" s="34" t="s">
+        <v>254</v>
+      </c>
+      <c r="S4" s="34" t="s">
+        <v>254</v>
+      </c>
+      <c r="T4" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="F5" s="33" t="s">
+        <v>239</v>
+      </c>
+      <c r="G5" s="33" t="s">
         <v>244</v>
       </c>
-      <c r="I4" t="s">
+      <c r="H5" t="s">
+        <v>354</v>
+      </c>
+      <c r="L5" s="35" t="s">
         <v>255</v>
       </c>
-      <c r="J4" s="32" t="s">
-        <v>239</v>
-      </c>
-      <c r="K4" s="33" t="s">
+      <c r="S5" s="34" t="s">
+        <v>256</v>
+      </c>
+      <c r="T5" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="F6" s="34" t="s">
         <v>240</v>
       </c>
-      <c r="L4" s="34" t="s">
+      <c r="G6" s="34" t="s">
+        <v>242</v>
+      </c>
+      <c r="H6" t="s">
+        <v>388</v>
+      </c>
+      <c r="K6" s="33" t="s">
+        <v>350</v>
+      </c>
+      <c r="L6" s="34" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="F5" s="33" t="s">
-        <v>240</v>
-      </c>
-      <c r="G5" s="33" t="s">
-        <v>245</v>
-      </c>
-      <c r="L5" s="35" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="F6" s="34" t="s">
-        <v>241</v>
-      </c>
-      <c r="G6" s="34" t="s">
-        <v>243</v>
-      </c>
-      <c r="K6" s="33" t="s">
-        <v>240</v>
-      </c>
-      <c r="L6" s="34" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S6" s="34" t="s">
+        <v>327</v>
+      </c>
+      <c r="T6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B7" s="12" t="s">
         <v>208</v>
       </c>
@@ -4713,16 +4968,25 @@
         <v>210</v>
       </c>
       <c r="F7" s="35" t="s">
+        <v>241</v>
+      </c>
+      <c r="G7" s="35" t="s">
         <v>242</v>
       </c>
-      <c r="G7" s="35" t="s">
-        <v>243</v>
+      <c r="H7" t="s">
+        <v>389</v>
       </c>
       <c r="L7" s="35" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+        <v>349</v>
+      </c>
+      <c r="S7" s="34" t="s">
+        <v>377</v>
+      </c>
+      <c r="T7" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>182</v>
       </c>
@@ -4733,16 +4997,22 @@
         <v>186</v>
       </c>
       <c r="K8" s="33" t="s">
-        <v>240</v>
+        <v>351</v>
       </c>
       <c r="L8" s="34" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="M8" s="34" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+        <v>347</v>
+      </c>
+      <c r="S8" s="34" t="s">
+        <v>257</v>
+      </c>
+      <c r="T8" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>176</v>
       </c>
@@ -4753,13 +5023,19 @@
         <v>187</v>
       </c>
       <c r="L9" s="35" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="M9" s="35" t="s">
+        <v>348</v>
+      </c>
+      <c r="S9" s="34" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="T9" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>182</v>
       </c>
@@ -4769,14 +5045,26 @@
       <c r="D10" t="s">
         <v>186</v>
       </c>
+      <c r="F10" t="s">
+        <v>395</v>
+      </c>
+      <c r="G10" t="s">
+        <v>397</v>
+      </c>
       <c r="K10" s="33" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L10" s="34" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+      <c r="S10" s="34" t="s">
+        <v>372</v>
+      </c>
+      <c r="T10" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>176</v>
       </c>
@@ -4786,22 +5074,46 @@
       <c r="D11" t="s">
         <v>187</v>
       </c>
+      <c r="F11" t="s">
+        <v>396</v>
+      </c>
+      <c r="G11" t="s">
+        <v>398</v>
+      </c>
       <c r="L11" s="32" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="M11" s="33" t="s">
-        <v>338</v>
+        <v>350</v>
       </c>
       <c r="N11" s="34" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="N12" s="34" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+        <v>357</v>
+      </c>
+      <c r="O11" t="s">
+        <v>371</v>
+      </c>
+      <c r="S11" s="34" t="s">
+        <v>358</v>
+      </c>
+      <c r="T11" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="N12" s="33" t="s">
+        <v>350</v>
+      </c>
+      <c r="O12" s="34" t="s">
+        <v>366</v>
+      </c>
+      <c r="S12" s="34" t="s">
+        <v>359</v>
+      </c>
+      <c r="T12" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>177</v>
       </c>
@@ -4809,38 +5121,44 @@
         <v>188</v>
       </c>
       <c r="D13" t="s">
-        <v>237</v>
-      </c>
-      <c r="N13" s="32" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="M14" s="35" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="K15" s="33" t="s">
-        <v>240</v>
-      </c>
-      <c r="L15" s="34" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+      <c r="O13" s="35" t="s">
+        <v>364</v>
+      </c>
+      <c r="S13" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="T13" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="O14" s="35" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="N15" s="33" t="s">
+        <v>350</v>
+      </c>
+      <c r="O15" s="34" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B16" s="12" t="s">
         <v>207</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
-      <c r="L16" s="35" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O16" s="35" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B17" t="s">
         <v>197</v>
@@ -4848,16 +5166,16 @@
       <c r="C17" t="s">
         <v>200</v>
       </c>
-      <c r="K17" s="33" t="s">
-        <v>240</v>
-      </c>
-      <c r="L17" s="34" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H17" t="s">
+        <v>394</v>
+      </c>
+      <c r="O17" s="35" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B18" t="s">
         <v>221</v>
@@ -4868,13 +5186,16 @@
       <c r="E18" t="s">
         <v>223</v>
       </c>
-      <c r="L18" s="35" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M18" s="33" t="s">
+        <v>239</v>
+      </c>
+      <c r="N18" s="34" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="38" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B19" s="38" t="s">
         <v>196</v>
@@ -4883,18 +5204,16 @@
         <v>199</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>335</v>
-      </c>
-      <c r="E19" s="43" t="s">
-        <v>224</v>
-      </c>
-      <c r="K19" s="35" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="E19" s="43"/>
+      <c r="N19" s="35" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="39" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B20" s="39" t="s">
         <v>203</v>
@@ -4904,10 +5223,16 @@
       </c>
       <c r="D20" s="39"/>
       <c r="E20" s="43"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M20" s="33" t="s">
+        <v>239</v>
+      </c>
+      <c r="N20" s="34" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="39" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B21" s="39" t="s">
         <v>205</v>
@@ -4917,10 +5242,16 @@
       </c>
       <c r="D21" s="39"/>
       <c r="E21" s="43"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N21" s="35" t="s">
+        <v>356</v>
+      </c>
+      <c r="T21" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="38" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B22" s="38" t="s">
         <v>212</v>
@@ -4930,25 +5261,49 @@
       </c>
       <c r="D22" s="38"/>
       <c r="E22" s="43"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N22" s="32" t="s">
+        <v>352</v>
+      </c>
+      <c r="O22" s="33" t="s">
+        <v>239</v>
+      </c>
+      <c r="P22" s="34" t="s">
+        <v>393</v>
+      </c>
+      <c r="S22" s="35" t="s">
+        <v>251</v>
+      </c>
+      <c r="T22" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="38" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C23" s="38" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="D23" s="38" t="s">
-        <v>337</v>
+        <v>370</v>
       </c>
       <c r="E23" s="43"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="P23" s="35" t="s">
+        <v>392</v>
+      </c>
+      <c r="S23" s="35" t="s">
+        <v>349</v>
+      </c>
+      <c r="T23" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B24" t="s">
         <v>201</v>
@@ -4957,12 +5312,21 @@
         <v>202</v>
       </c>
       <c r="E24" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+      <c r="O24" s="35" t="s">
+        <v>374</v>
+      </c>
+      <c r="S24" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="T24" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B25" t="s">
         <v>198</v>
@@ -4971,31 +5335,70 @@
         <v>211</v>
       </c>
       <c r="E25" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+      <c r="M25" s="35" t="s">
+        <v>376</v>
+      </c>
+      <c r="S25" s="35" t="s">
+        <v>355</v>
+      </c>
+      <c r="T25" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K26" s="33" t="s">
+        <v>239</v>
+      </c>
+      <c r="L26" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="S26" s="35" t="s">
+        <v>356</v>
+      </c>
+      <c r="T26" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>215</v>
       </c>
       <c r="C27" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L27" s="35" t="s">
+        <v>252</v>
+      </c>
+      <c r="S27" s="35" t="s">
+        <v>248</v>
+      </c>
+      <c r="T27" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>217</v>
       </c>
       <c r="C28" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K28" s="35" t="s">
+        <v>259</v>
+      </c>
+      <c r="S28" s="35" t="s">
+        <v>249</v>
+      </c>
+      <c r="T28" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>219</v>
       </c>
@@ -5003,7 +5406,10 @@
         <v>220</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S31" s="44"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>189</v>
       </c>
@@ -5012,6 +5418,9 @@
       </c>
       <c r="D32" t="s">
         <v>191</v>
+      </c>
+      <c r="I32" s="45" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.2">
@@ -5044,399 +5453,399 @@
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C39" t="s">
+        <v>226</v>
+      </c>
+      <c r="D39" t="s">
         <v>227</v>
-      </c>
-      <c r="D39" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D40" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C41" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D41" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C42" t="s">
+        <v>232</v>
+      </c>
+      <c r="D42" t="s">
         <v>233</v>
-      </c>
-      <c r="D42" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C43" t="s">
+        <v>234</v>
+      </c>
+      <c r="D43" t="s">
         <v>235</v>
-      </c>
-      <c r="D43" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C44" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D44" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="H44" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="I44" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="J44" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="K44" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="L44" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.2">
       <c r="F45" s="36"/>
       <c r="G45" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="H45" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="I45" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="J45" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="K45" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="L45" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.2">
       <c r="F46" s="36"/>
       <c r="G46" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="H46" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="I46" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="J46" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="K46" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="L46" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="F47" s="36"/>
       <c r="G47" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="H47" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="I47" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="J47" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="K47" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="L47" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F48" s="36"/>
       <c r="G48" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="H48" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="I48" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="J48" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="K48" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="L48" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="49" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F49" s="36"/>
       <c r="G49" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="H49" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="I49" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="J49" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="K49" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="L49" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
     </row>
     <row r="50" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F50" s="36"/>
       <c r="G50" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="H50" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="I50" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="J50" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="K50" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="L50" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
     </row>
     <row r="51" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F51" s="36"/>
       <c r="G51" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="H51" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="I51" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="J51" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="K51" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="L51" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="52" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F52" s="36"/>
       <c r="G52" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="H52" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="I52" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="J52" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="K52" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="L52" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
     <row r="53" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F53" s="36"/>
       <c r="G53" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="H53" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="I53" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="J53" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="K53" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="L53" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="62" spans="6:14" x14ac:dyDescent="0.2">
       <c r="H62" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="J62" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="L62" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="N62" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
     </row>
     <row r="63" spans="6:14" ht="57" x14ac:dyDescent="0.2">
       <c r="G63" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="H63" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="I63" s="37" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="J63" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="L63" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="M63" s="37" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
     </row>
     <row r="64" spans="6:14" x14ac:dyDescent="0.2">
       <c r="G64" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="H64" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="I64" s="37"/>
       <c r="L64" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="M64" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
     </row>
     <row r="65" spans="7:13" x14ac:dyDescent="0.2">
       <c r="G65" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="H65" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="I65" s="37"/>
       <c r="L65" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="M65" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="66" spans="7:13" x14ac:dyDescent="0.2">
       <c r="G66" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="H66" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="I66" s="37"/>
       <c r="L66" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="M66" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
     </row>
     <row r="67" spans="7:13" x14ac:dyDescent="0.2">
       <c r="G67" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="H67" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="I67" s="37" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="L67" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="M67" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="68" spans="7:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="G68" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="H68" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="I68" s="37" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="L68" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="M68" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
     </row>
     <row r="69" spans="7:13" x14ac:dyDescent="0.2">
       <c r="G69" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="I69" s="37"/>
       <c r="L69" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="M69" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="70" spans="7:13" x14ac:dyDescent="0.2">
       <c r="G70" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="I70" s="37"/>
     </row>
     <row r="71" spans="7:13" x14ac:dyDescent="0.2">
       <c r="G71" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="I71" s="37"/>
     </row>
@@ -5447,6 +5856,7 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Ver 0.0.0005   todo: item & equip.
</commit_message>
<xml_diff>
--- a/数值表.xlsx
+++ b/数值表.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12240" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12240" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Roles" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="427">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1650,6 +1650,70 @@
   </si>
   <si>
     <t>得高人传授的宝物, 内有乾坤, 可容纳海量物品(背包)….</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击动画时间和间隔, 与攻速相关联</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击范围</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单体</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直线</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>扇形</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>十字型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本地圆形</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>目标圆形</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自身(无)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>施法动作1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击动作1/2随机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能范围提示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>实际影响效果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>粒子效果</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2384,7 +2448,7 @@
   <dimension ref="A1:U52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2951,8 +3015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3886,10 +3950,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K40"/>
+  <dimension ref="B2:Q40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:K13"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3901,7 +3965,7 @@
     <col min="6" max="16384" width="9" style="14"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
       <c r="F2" s="42" t="s">
         <v>75</v>
       </c>
@@ -3913,7 +3977,7 @@
       <c r="J2" s="42"/>
       <c r="K2" s="42"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B3" s="15" t="s">
         <v>68</v>
       </c>
@@ -3944,116 +4008,167 @@
       <c r="K3" s="19" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L3" s="14" t="s">
+        <v>414</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B4" s="25">
         <v>1</v>
       </c>
+      <c r="C4" s="14" t="s">
+        <v>411</v>
+      </c>
       <c r="D4" s="14" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="E4" s="14">
+        <v>0</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>415</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>423</v>
+      </c>
+      <c r="Q4" s="14" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B5" s="25">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B6" s="25">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B7" s="25">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L7" s="14" t="s">
+        <v>421</v>
+      </c>
+      <c r="N7" s="14" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B8" s="25">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B9" s="25">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B10" s="25">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B11" s="25">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L11" s="14" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B12" s="25">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B13" s="25">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B14" s="25">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L14" s="14" t="s">
+        <v>417</v>
+      </c>
+      <c r="N14" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="O14" s="14" t="s">
+        <v>425</v>
+      </c>
+      <c r="P14" s="14" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B15" s="25">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B16" s="25">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17" s="25">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="L17" s="14" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18" s="25">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B19" s="25">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B20" s="25">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="L20" s="14" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" s="25">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B22" s="25">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" s="25">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B24" s="25">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="L24" s="14" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B25" s="25">
         <v>22</v>
       </c>
@@ -4073,37 +4188,37 @@
         <v>148</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B26" s="25">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B27" s="25">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B28" s="25">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B29" s="25">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B30" s="25">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B31" s="25">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B32" s="25">
         <v>29</v>
       </c>
@@ -4130,6 +4245,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4137,7 +4253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K53"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
@@ -4780,7 +4896,7 @@
   <dimension ref="A2:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5015,8 +5131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T71"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Ver 0.0.0006   todo: how to split iteminfo by itemtype, and don't influence grid's and inventory's function?
</commit_message>
<xml_diff>
--- a/数值表.xlsx
+++ b/数值表.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12240" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12240" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Roles" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="449">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1714,6 +1714,93 @@
   </si>
   <si>
     <t>粒子效果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消耗品</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蜡杆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>材料</t>
+  </si>
+  <si>
+    <t>背包</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>装备栏</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>格子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>物品</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>物品信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>武器栏</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>护甲栏</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>饰品栏1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>饰品栏2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>很多</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>格子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4个</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>筛选</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>武器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>护甲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>饰品</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消耗品</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>素材</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>任务品</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3013,10 +3100,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N44"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3393,65 +3480,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>51</v>
-      </c>
-      <c r="B35" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" t="s">
-        <v>11</v>
-      </c>
-      <c r="H35" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>52</v>
-      </c>
-      <c r="B36" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" t="s">
-        <v>11</v>
-      </c>
-      <c r="H36" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>53</v>
-      </c>
-      <c r="B37" t="s">
-        <v>40</v>
-      </c>
-      <c r="C37" t="s">
-        <v>11</v>
-      </c>
-      <c r="G37" t="s">
-        <v>42</v>
-      </c>
-      <c r="H37" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>54</v>
-      </c>
-      <c r="B38" t="s">
-        <v>41</v>
-      </c>
-      <c r="C38" t="s">
-        <v>11</v>
-      </c>
-      <c r="H38" t="s">
-        <v>51</v>
-      </c>
-    </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>100</v>
@@ -3466,11 +3494,85 @@
         <v>410</v>
       </c>
     </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>101</v>
+      </c>
+      <c r="B45" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>102</v>
+      </c>
+      <c r="B46" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" t="s">
+        <v>11</v>
+      </c>
+      <c r="H46" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>103</v>
+      </c>
+      <c r="B47" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" t="s">
+        <v>42</v>
+      </c>
+      <c r="H47" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>104</v>
+      </c>
+      <c r="B48" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48" t="s">
+        <v>11</v>
+      </c>
+      <c r="H48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>200</v>
+      </c>
+      <c r="B52" t="s">
+        <v>428</v>
+      </c>
+      <c r="C52" t="s">
+        <v>429</v>
+      </c>
+    </row>
   </sheetData>
+  <dataConsolidate/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C1048576 C1">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1 C116:C1048576 C3">
       <formula1>$N$3:$N$8</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C115">
+      <formula1>$N$3:$N$9</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3480,10 +3582,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:J35"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3491,7 +3593,12 @@
     <col min="3" max="3" width="9" style="14"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B3" s="25"/>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -3501,7 +3608,7 @@
       <c r="I3" s="14"/>
       <c r="J3" s="14"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B4" s="25"/>
       <c r="D4" s="14"/>
       <c r="E4" s="42" t="s">
@@ -3515,7 +3622,7 @@
       <c r="I4" s="42"/>
       <c r="J4" s="42"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" s="16" t="s">
         <v>68</v>
       </c>
@@ -3544,7 +3651,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6" s="25">
         <v>1</v>
       </c>
@@ -3559,7 +3666,7 @@
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B7" s="25">
         <v>2</v>
       </c>
@@ -3574,7 +3681,7 @@
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B8" s="25">
         <v>3</v>
       </c>
@@ -3589,7 +3696,7 @@
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9" s="25">
         <v>4</v>
       </c>
@@ -3604,7 +3711,7 @@
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B10" s="25">
         <v>5</v>
       </c>
@@ -3619,7 +3726,7 @@
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11" s="25">
         <v>6</v>
       </c>
@@ -3634,7 +3741,7 @@
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" s="25">
         <v>7</v>
       </c>
@@ -3646,7 +3753,7 @@
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" s="25">
         <v>8</v>
       </c>
@@ -3658,7 +3765,7 @@
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14" s="25">
         <v>9</v>
       </c>
@@ -3670,7 +3777,7 @@
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15" s="25">
         <v>10</v>
       </c>
@@ -3682,7 +3789,7 @@
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16" s="25">
         <v>11</v>
       </c>
@@ -3825,20 +3932,11 @@
       <c r="B27" s="25">
         <v>22</v>
       </c>
-      <c r="C27" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="D27" s="14">
-        <v>30</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>147</v>
-      </c>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
-      <c r="H27" s="14" t="s">
-        <v>148</v>
-      </c>
+      <c r="H27" s="14"/>
       <c r="I27" s="14"/>
       <c r="J27" s="14"/>
     </row>
@@ -5131,8 +5229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6165,12 +6263,96 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="D7:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="7" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>430</v>
+      </c>
+      <c r="F7" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="8" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>442</v>
+      </c>
+      <c r="F8" t="s">
+        <v>435</v>
+      </c>
+      <c r="G8" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="9" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>436</v>
+      </c>
+      <c r="G9" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="10" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>432</v>
+      </c>
+      <c r="E10" t="s">
+        <v>439</v>
+      </c>
+      <c r="F10" t="s">
+        <v>440</v>
+      </c>
+      <c r="G10" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="13" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="15" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="16" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>448</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ver 0.0.0011 item roughly finished.. todo: text and icons about skill/item/buff/effect..
</commit_message>
<xml_diff>
--- a/数值表.xlsx
+++ b/数值表.xlsx
@@ -2480,6 +2480,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2490,9 +2493,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3395,8 +3395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4180,16 +4180,16 @@
       <c r="A77" s="24" t="s">
         <v>434</v>
       </c>
-      <c r="D77" s="42" t="s">
+      <c r="D77" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="E77" s="42"/>
-      <c r="F77" s="42"/>
-      <c r="G77" s="42" t="s">
+      <c r="E77" s="43"/>
+      <c r="F77" s="43"/>
+      <c r="G77" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="H77" s="42"/>
-      <c r="I77" s="42"/>
+      <c r="H77" s="43"/>
+      <c r="I77" s="43"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" s="41" t="s">
@@ -4219,7 +4219,7 @@
       <c r="I78" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="J78" s="46" t="s">
+      <c r="J78" s="42" t="s">
         <v>453</v>
       </c>
     </row>
@@ -4650,16 +4650,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="F2" s="42" t="s">
+      <c r="F2" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42" t="s">
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B3" s="15" t="s">
@@ -4960,18 +4960,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="E2" s="43" t="s">
+      <c r="E2" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="43" t="s">
+      <c r="F2" s="45"/>
+      <c r="G2" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="H2" s="44"/>
-      <c r="I2" s="43" t="s">
+      <c r="H2" s="45"/>
+      <c r="I2" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="J2" s="44"/>
+      <c r="J2" s="45"/>
       <c r="K2" s="14" t="s">
         <v>135</v>
       </c>
@@ -6193,7 +6193,7 @@
       <c r="D19" s="37" t="s">
         <v>301</v>
       </c>
-      <c r="E19" s="45"/>
+      <c r="E19" s="46"/>
       <c r="N19" s="34" t="s">
         <v>219</v>
       </c>
@@ -6209,7 +6209,7 @@
         <v>175</v>
       </c>
       <c r="D20" s="38"/>
-      <c r="E20" s="45"/>
+      <c r="E20" s="46"/>
       <c r="M20" s="32" t="s">
         <v>210</v>
       </c>
@@ -6228,7 +6228,7 @@
         <v>177</v>
       </c>
       <c r="D21" s="38"/>
-      <c r="E21" s="45"/>
+      <c r="E21" s="46"/>
       <c r="N21" s="34" t="s">
         <v>327</v>
       </c>
@@ -6247,7 +6247,7 @@
         <v>184</v>
       </c>
       <c r="D22" s="37"/>
-      <c r="E22" s="45"/>
+      <c r="E22" s="46"/>
       <c r="N22" s="31" t="s">
         <v>323</v>
       </c>
@@ -6277,7 +6277,7 @@
       <c r="D23" s="37" t="s">
         <v>341</v>
       </c>
-      <c r="E23" s="45"/>
+      <c r="E23" s="46"/>
       <c r="P23" s="34" t="s">
         <v>363</v>
       </c>

</xml_diff>

<commit_message>
Ver 0.0.0014 ai test & dropout item.
</commit_message>
<xml_diff>
--- a/数值表.xlsx
+++ b/数值表.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="676">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -500,14 +500,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>腾龙</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>畏惧</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>我</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2669,6 +2661,33 @@
   </si>
   <si>
     <t>player镜像</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>暴怒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>敌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>暴怒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>溃散</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ManaDamage</t>
+  </si>
+  <si>
+    <t>ManaDamage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MP伤害</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3557,7 +3576,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>9</v>
@@ -3566,7 +3585,7 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="M4" t="s">
         <v>19</v>
@@ -3580,7 +3599,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>9</v>
@@ -3589,7 +3608,7 @@
         <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="M5" t="s">
         <v>13</v>
@@ -3603,7 +3622,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>9</v>
@@ -3612,7 +3631,7 @@
         <v>3</v>
       </c>
       <c r="H6" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="M6" t="s">
         <v>17</v>
@@ -3626,7 +3645,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>9</v>
@@ -3635,7 +3654,7 @@
         <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="M7" t="s">
         <v>4</v>
@@ -3649,7 +3668,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>9</v>
@@ -3658,7 +3677,7 @@
         <v>5</v>
       </c>
       <c r="H8" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="M8" t="s">
         <v>5</v>
@@ -3672,7 +3691,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>9</v>
@@ -3681,13 +3700,13 @@
         <v>6</v>
       </c>
       <c r="H9" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="M9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -3695,7 +3714,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>9</v>
@@ -3704,7 +3723,7 @@
         <v>7</v>
       </c>
       <c r="H10" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -3712,7 +3731,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>9</v>
@@ -3721,7 +3740,7 @@
         <v>8</v>
       </c>
       <c r="H11" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -3729,7 +3748,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>9</v>
@@ -3738,10 +3757,10 @@
         <v>9</v>
       </c>
       <c r="G12" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="H12" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -3749,16 +3768,16 @@
         <v>10</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>9</v>
       </c>
       <c r="G13" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="H13" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -3766,16 +3785,16 @@
         <v>11</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>9</v>
       </c>
       <c r="G14" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="H14" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -3783,16 +3802,16 @@
         <v>12</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>9</v>
       </c>
       <c r="G15" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="H15" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -3800,16 +3819,16 @@
         <v>13</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>9</v>
       </c>
       <c r="G16" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="H16" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
@@ -3817,16 +3836,16 @@
         <v>14</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>9</v>
       </c>
       <c r="G17" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="H17" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
@@ -3843,10 +3862,10 @@
         <v>10</v>
       </c>
       <c r="G18" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="H18" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
@@ -3863,10 +3882,10 @@
         <v>10</v>
       </c>
       <c r="G19" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="H19" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.2">
@@ -3883,10 +3902,10 @@
         <v>100</v>
       </c>
       <c r="G20" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="H20" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.2">
@@ -3903,10 +3922,10 @@
         <v>40</v>
       </c>
       <c r="G21" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="H21" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.2">
@@ -3923,37 +3942,37 @@
         <v>10</v>
       </c>
       <c r="G22" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="H22" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="K22" t="s">
+        <v>662</v>
+      </c>
+      <c r="M22" t="s">
+        <v>654</v>
+      </c>
+      <c r="N22" t="s">
+        <v>655</v>
+      </c>
+      <c r="O22" t="s">
+        <v>656</v>
+      </c>
+      <c r="P22" t="s">
+        <v>657</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>658</v>
+      </c>
+      <c r="R22" t="s">
+        <v>659</v>
+      </c>
+      <c r="S22" s="2" t="s">
         <v>664</v>
       </c>
-      <c r="M22" t="s">
-        <v>656</v>
-      </c>
-      <c r="N22" t="s">
-        <v>657</v>
-      </c>
-      <c r="O22" t="s">
-        <v>658</v>
-      </c>
-      <c r="P22" t="s">
-        <v>659</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>660</v>
-      </c>
-      <c r="R22" t="s">
-        <v>661</v>
-      </c>
-      <c r="S22" s="2" t="s">
-        <v>666</v>
-      </c>
       <c r="T22" s="63" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="U22" s="63"/>
       <c r="V22" s="63"/>
@@ -3963,13 +3982,13 @@
         <v>20</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>14</v>
       </c>
       <c r="H23" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="K23">
         <v>1</v>
@@ -4021,7 +4040,7 @@
         <v>14</v>
       </c>
       <c r="H24" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="K24">
         <v>10</v>
@@ -4073,7 +4092,7 @@
         <v>14</v>
       </c>
       <c r="H25" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="K25">
         <v>19</v>
@@ -4116,13 +4135,13 @@
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B26" s="14" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>14</v>
       </c>
       <c r="H26" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="K26">
         <v>28</v>
@@ -4174,10 +4193,10 @@
         <v>14</v>
       </c>
       <c r="G27" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="H27" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="K27">
         <v>37</v>
@@ -4223,16 +4242,16 @@
         <v>24</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G28" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="H28" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="K28">
         <v>46</v>
@@ -4278,16 +4297,16 @@
         <v>25</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G29" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="H29" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="K29">
         <v>46</v>
@@ -4333,13 +4352,13 @@
         <v>26</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>16</v>
       </c>
       <c r="H30" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="K30">
         <v>1</v>
@@ -4362,13 +4381,13 @@
         <v>27</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="C31" s="14" t="s">
         <v>16</v>
       </c>
       <c r="H31" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="K31">
         <v>10</v>
@@ -4391,13 +4410,13 @@
         <v>28</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="H32" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="K32">
         <v>19</v>
@@ -4426,7 +4445,7 @@
         <v>16</v>
       </c>
       <c r="H33" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="K33">
         <v>28</v>
@@ -4455,10 +4474,10 @@
         <v>16</v>
       </c>
       <c r="G34" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="H34" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="K34">
         <v>37</v>
@@ -4481,16 +4500,16 @@
         <v>31</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C35" s="14" t="s">
         <v>16</v>
       </c>
       <c r="G35" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="H35" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="K35">
         <v>46</v>
@@ -4513,16 +4532,16 @@
         <v>32</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="C36" s="14" t="s">
         <v>16</v>
       </c>
       <c r="G36" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="H36" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="K36">
         <v>46</v>
@@ -4545,16 +4564,16 @@
         <v>33</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="C37" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G37" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="H37" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.2">
@@ -4568,10 +4587,10 @@
         <v>7</v>
       </c>
       <c r="G38" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="H38" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.2">
@@ -4585,10 +4604,10 @@
         <v>7</v>
       </c>
       <c r="G39" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="H39" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.2">
@@ -4602,10 +4621,10 @@
         <v>7</v>
       </c>
       <c r="G40" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H40" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.2">
@@ -4613,16 +4632,16 @@
         <v>37</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C41" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G41" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="H41" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.2">
@@ -4630,16 +4649,16 @@
         <v>38</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C42" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G42" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="H42" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.2">
@@ -4647,16 +4666,16 @@
         <v>39</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="C43" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G43" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="H43" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.2">
@@ -4670,10 +4689,10 @@
         <v>7</v>
       </c>
       <c r="G44" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="H44" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.2">
@@ -4681,16 +4700,16 @@
         <v>41</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="C45" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G45" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="H45" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.2">
@@ -4698,16 +4717,16 @@
         <v>42</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="C46" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G46" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="H46" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.2">
@@ -4715,13 +4734,13 @@
         <v>43</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C47" s="14" t="s">
         <v>11</v>
       </c>
       <c r="H47" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -4793,15 +4812,15 @@
         <v>200</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" s="21" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D78" s="62" t="s">
         <v>64</v>
@@ -4843,7 +4862,7 @@
         <v>62</v>
       </c>
       <c r="J79" s="36" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.2">
@@ -4851,7 +4870,7 @@
         <v>1</v>
       </c>
       <c r="B80" s="14" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D80" s="14"/>
       <c r="E80" s="14"/>
@@ -4860,13 +4879,13 @@
       <c r="H80" s="14"/>
       <c r="I80" s="14"/>
       <c r="J80" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="K80" t="s">
+        <v>422</v>
+      </c>
+      <c r="L80" t="s">
         <v>433</v>
-      </c>
-      <c r="K80" t="s">
-        <v>424</v>
-      </c>
-      <c r="L80" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.2">
@@ -4874,7 +4893,7 @@
         <v>2</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D81" s="14"/>
       <c r="E81" s="14"/>
@@ -4883,13 +4902,13 @@
       <c r="H81" s="14"/>
       <c r="I81" s="14"/>
       <c r="J81" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="K81" t="s">
+        <v>423</v>
+      </c>
+      <c r="L81" t="s">
         <v>425</v>
-      </c>
-      <c r="L81" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.2">
@@ -4897,7 +4916,7 @@
         <v>3</v>
       </c>
       <c r="B82" s="14" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D82" s="14"/>
       <c r="E82" s="14"/>
@@ -4906,13 +4925,13 @@
       <c r="H82" s="14"/>
       <c r="I82" s="14"/>
       <c r="J82" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="K82" t="s">
+        <v>424</v>
+      </c>
+      <c r="L82" t="s">
         <v>434</v>
-      </c>
-      <c r="K82" t="s">
-        <v>426</v>
-      </c>
-      <c r="L82" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.2">
@@ -4920,7 +4939,7 @@
         <v>4</v>
       </c>
       <c r="B83" s="14" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D83" s="14"/>
       <c r="E83" s="14"/>
@@ -4934,7 +4953,7 @@
         <v>5</v>
       </c>
       <c r="B84" s="14" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D84" s="14"/>
       <c r="E84" s="14"/>
@@ -4948,7 +4967,7 @@
         <v>6</v>
       </c>
       <c r="B85" s="14" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D85" s="14"/>
       <c r="E85" s="14"/>
@@ -4962,7 +4981,7 @@
         <v>7</v>
       </c>
       <c r="B86" s="14" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D86" s="14"/>
       <c r="E86" s="14"/>
@@ -4976,7 +4995,7 @@
         <v>8</v>
       </c>
       <c r="B87" s="14" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D87" s="14"/>
       <c r="E87" s="14"/>
@@ -4990,7 +5009,7 @@
         <v>9</v>
       </c>
       <c r="B88" s="14" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D88" s="14"/>
       <c r="E88" s="14"/>
@@ -5015,13 +5034,13 @@
         <v>11</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D90" s="14"/>
       <c r="E90" s="14"/>
       <c r="F90" s="14"/>
       <c r="G90" s="14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H90" s="14"/>
       <c r="I90" s="14"/>
@@ -5260,8 +5279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5291,7 +5310,7 @@
       <c r="T1" s="6"/>
       <c r="U1" s="6"/>
       <c r="V1" s="6" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="W1" s="7"/>
     </row>
@@ -5328,28 +5347,28 @@
         <v>50</v>
       </c>
       <c r="X2" s="23" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="Y2" s="23" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="AA2" s="23" t="s">
+        <v>626</v>
+      </c>
+      <c r="AB2" s="23" t="s">
+        <v>629</v>
+      </c>
+      <c r="AC2" s="23" t="s">
+        <v>627</v>
+      </c>
+      <c r="AD2" s="23" t="s">
+        <v>627</v>
+      </c>
+      <c r="AE2" s="23" t="s">
         <v>628</v>
       </c>
-      <c r="AB2" s="23" t="s">
-        <v>631</v>
-      </c>
-      <c r="AC2" s="23" t="s">
-        <v>629</v>
-      </c>
-      <c r="AD2" s="23" t="s">
-        <v>629</v>
-      </c>
-      <c r="AE2" s="23" t="s">
+      <c r="AF2" s="23" t="s">
         <v>630</v>
-      </c>
-      <c r="AF2" s="23" t="s">
-        <v>632</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.2">
@@ -5564,22 +5583,22 @@
         <v>47</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>364</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>365</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>366</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="I6" s="52" t="s">
         <v>367</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>368</v>
-      </c>
-      <c r="I6" s="52" t="s">
-        <v>369</v>
       </c>
       <c r="K6" s="51"/>
       <c r="L6" s="9"/>
@@ -5651,22 +5670,22 @@
         <v>48</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E7" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="G7" s="12" t="s">
         <v>359</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="H7" s="12" t="s">
         <v>360</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="I7" s="53" t="s">
         <v>361</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>362</v>
-      </c>
-      <c r="I7" s="53" t="s">
-        <v>363</v>
       </c>
       <c r="K7" s="51"/>
       <c r="L7" s="9"/>
@@ -6011,7 +6030,7 @@
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="64" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D12" s="64"/>
       <c r="F12">
@@ -6170,20 +6189,20 @@
       <c r="C14" s="12"/>
       <c r="D14" s="13"/>
       <c r="E14" t="s">
+        <v>631</v>
+      </c>
+      <c r="G14" t="s">
+        <v>632</v>
+      </c>
+      <c r="I14" s="14" t="s">
         <v>633</v>
       </c>
-      <c r="G14" t="s">
+      <c r="K14" s="51" t="s">
         <v>634</v>
-      </c>
-      <c r="I14" s="14" t="s">
-        <v>635</v>
-      </c>
-      <c r="K14" s="51" t="s">
-        <v>636</v>
       </c>
       <c r="L14" s="9"/>
       <c r="M14" s="54" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="N14" s="9"/>
       <c r="O14" s="3">
@@ -6249,13 +6268,13 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C15" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D15" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="K15" s="51"/>
       <c r="L15" s="9"/>
@@ -6327,10 +6346,10 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D16" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="K16" s="51"/>
       <c r="L16" s="9"/>
@@ -6402,7 +6421,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="K17" s="51"/>
       <c r="L17" s="9"/>
@@ -6474,7 +6493,7 @@
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="K18" s="51"/>
       <c r="L18" s="9"/>
@@ -6546,7 +6565,7 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="K19" s="51"/>
       <c r="L19" s="9"/>
@@ -6618,7 +6637,7 @@
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="K20" s="51"/>
       <c r="L20" s="9"/>
@@ -6690,7 +6709,7 @@
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="K21" s="51"/>
       <c r="L21" s="9"/>
@@ -7659,13 +7678,13 @@
         <v>20</v>
       </c>
       <c r="C35" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="E35" s="61">
         <v>10000</v>
       </c>
       <c r="F35" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -7683,7 +7702,7 @@
         <v>10</v>
       </c>
       <c r="L35" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="M35" s="51">
         <v>0</v>
@@ -7757,13 +7776,13 @@
         <v>21</v>
       </c>
       <c r="C36" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E36" s="14">
         <v>100</v>
       </c>
       <c r="F36" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="G36">
         <v>100</v>
@@ -7775,19 +7794,19 @@
         <v>8</v>
       </c>
       <c r="J36" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="K36" s="51">
         <v>12</v>
       </c>
       <c r="L36" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="M36" s="51">
         <v>10</v>
       </c>
       <c r="N36" s="9" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="O36" s="3">
         <v>34</v>
@@ -7855,13 +7874,13 @@
         <v>22</v>
       </c>
       <c r="C37" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E37" s="14">
         <v>100</v>
       </c>
       <c r="F37" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="G37">
         <v>100</v>
@@ -7873,19 +7892,19 @@
         <v>9</v>
       </c>
       <c r="J37" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="K37" s="51">
         <v>9</v>
       </c>
       <c r="L37" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="M37" s="51">
         <v>10</v>
       </c>
       <c r="N37" s="9" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="O37" s="3">
         <v>35</v>
@@ -7953,13 +7972,13 @@
         <v>23</v>
       </c>
       <c r="C38" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E38" s="14">
         <v>100</v>
       </c>
       <c r="F38" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="G38">
         <v>100</v>
@@ -7971,19 +7990,19 @@
         <v>10</v>
       </c>
       <c r="J38" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="K38" s="51">
         <v>10</v>
       </c>
       <c r="L38" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="M38" s="51">
         <v>11</v>
       </c>
       <c r="N38" s="9" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="O38" s="3">
         <v>36</v>
@@ -8051,13 +8070,13 @@
         <v>24</v>
       </c>
       <c r="C39" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E39" s="14">
         <v>80</v>
       </c>
       <c r="F39" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="G39">
         <v>100</v>
@@ -8069,19 +8088,19 @@
         <v>8</v>
       </c>
       <c r="J39" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="K39" s="51">
         <v>8</v>
       </c>
       <c r="L39" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="M39" s="54">
         <v>9</v>
       </c>
       <c r="N39" s="9" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="O39" s="3">
         <v>37</v>
@@ -8149,13 +8168,13 @@
         <v>25</v>
       </c>
       <c r="C40" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E40" s="14">
         <v>80</v>
       </c>
       <c r="F40" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="G40">
         <v>100</v>
@@ -8167,19 +8186,19 @@
         <v>10</v>
       </c>
       <c r="J40" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="K40" s="51">
         <v>8</v>
       </c>
       <c r="L40" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="M40" s="54">
         <v>9</v>
       </c>
       <c r="N40" s="9" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="O40" s="3">
         <v>38</v>
@@ -8247,13 +8266,13 @@
         <v>26</v>
       </c>
       <c r="C41" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E41" s="14">
         <v>120</v>
       </c>
       <c r="F41" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="G41">
         <v>100</v>
@@ -8265,19 +8284,19 @@
         <v>12</v>
       </c>
       <c r="J41" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="K41" s="51">
         <v>10</v>
       </c>
       <c r="L41" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="M41" s="51">
         <v>15</v>
       </c>
       <c r="N41" s="9" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="O41" s="3">
         <v>39</v>
@@ -8345,13 +8364,13 @@
         <v>27</v>
       </c>
       <c r="C42" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E42" s="14">
         <v>110</v>
       </c>
       <c r="F42" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="G42">
         <v>100</v>
@@ -8363,19 +8382,19 @@
         <v>11</v>
       </c>
       <c r="J42" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="K42" s="51">
         <v>10</v>
       </c>
       <c r="L42" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="M42" s="51">
         <v>15</v>
       </c>
       <c r="N42" s="9" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="O42" s="3">
         <v>40</v>
@@ -8443,13 +8462,13 @@
         <v>28</v>
       </c>
       <c r="C43" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E43" s="14">
         <v>180</v>
       </c>
       <c r="F43" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="G43">
         <v>100</v>
@@ -8461,19 +8480,19 @@
         <v>18</v>
       </c>
       <c r="J43" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="K43" s="51">
         <v>15</v>
       </c>
       <c r="L43" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="M43" s="51">
         <v>20</v>
       </c>
       <c r="N43" s="9" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="O43" s="3">
         <v>41</v>
@@ -8541,13 +8560,13 @@
         <v>29</v>
       </c>
       <c r="C44" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E44" s="14">
         <v>150</v>
       </c>
       <c r="F44" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="G44">
         <v>100</v>
@@ -8559,19 +8578,19 @@
         <v>15</v>
       </c>
       <c r="J44" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="K44" s="51">
         <v>15</v>
       </c>
       <c r="L44" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="M44" s="51">
         <v>20</v>
       </c>
       <c r="N44" s="9" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="O44" s="3">
         <v>42</v>
@@ -8639,10 +8658,10 @@
         <v>30</v>
       </c>
       <c r="C45" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="D45" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="K45" s="51"/>
       <c r="L45" s="9"/>
@@ -9217,16 +9236,16 @@
     </row>
     <row r="56" spans="5:32" x14ac:dyDescent="0.2">
       <c r="E56" t="s">
+        <v>582</v>
+      </c>
+      <c r="F56" t="s">
+        <v>583</v>
+      </c>
+      <c r="G56" t="s">
         <v>584</v>
       </c>
-      <c r="F56" t="s">
+      <c r="H56" t="s">
         <v>585</v>
-      </c>
-      <c r="G56" t="s">
-        <v>586</v>
-      </c>
-      <c r="H56" t="s">
-        <v>587</v>
       </c>
       <c r="K56" s="51"/>
       <c r="L56" s="9"/>
@@ -10664,7 +10683,7 @@
   <dimension ref="B2:O53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -10716,7 +10735,7 @@
         <v>111</v>
       </c>
       <c r="F3" s="42" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="G3" s="41" t="s">
         <v>112</v>
@@ -10731,10 +10750,10 @@
         <v>109</v>
       </c>
       <c r="N3" s="37" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="O3" s="37" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.2">
@@ -10742,7 +10761,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D4" s="43">
         <v>20</v>
@@ -10763,13 +10782,13 @@
         <v>89</v>
       </c>
       <c r="K4" s="37" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="L4" s="37" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="M4" s="37" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="N4" s="37">
         <f>H4*D4+F4</f>
@@ -10784,7 +10803,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D5" s="46">
         <v>25</v>
@@ -10814,7 +10833,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D6" s="46">
         <v>30</v>
@@ -10844,7 +10863,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D7" s="46">
         <v>5</v>
@@ -10863,10 +10882,10 @@
         <v>89</v>
       </c>
       <c r="K7" s="37" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="L7" s="37" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="N7" s="37">
         <f>F7*D7</f>
@@ -10878,7 +10897,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D8" s="46">
         <v>6</v>
@@ -10934,7 +10953,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D10" s="46">
         <v>9</v>
@@ -10946,25 +10965,25 @@
         <v>50</v>
       </c>
       <c r="G10" s="44" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="H10" s="45">
         <v>50</v>
       </c>
       <c r="I10" s="44" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="J10" s="45">
         <v>15</v>
       </c>
       <c r="K10" s="37" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="L10" s="37" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="M10" s="37" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="N10" s="37">
         <f>F10</f>
@@ -10980,7 +10999,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D11" s="46">
         <v>12</v>
@@ -10992,13 +11011,13 @@
         <v>75</v>
       </c>
       <c r="G11" s="44" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="H11" s="45">
         <v>75</v>
       </c>
       <c r="I11" s="44" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="J11" s="45">
         <v>20</v>
@@ -11017,7 +11036,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D12" s="46">
         <v>15</v>
@@ -11029,13 +11048,13 @@
         <v>100</v>
       </c>
       <c r="G12" s="44" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="H12" s="45">
         <v>100</v>
       </c>
       <c r="I12" s="44" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="J12" s="45">
         <v>25</v>
@@ -11124,7 +11143,7 @@
         <v>20</v>
       </c>
       <c r="C23" s="38" t="s">
-        <v>123</v>
+        <v>671</v>
       </c>
       <c r="D23" s="43">
         <v>10</v>
@@ -11133,13 +11152,19 @@
         <v>69</v>
       </c>
       <c r="F23" s="45">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G23" s="44" t="s">
         <v>73</v>
       </c>
       <c r="H23" s="45">
-        <v>2</v>
+        <v>30</v>
+      </c>
+      <c r="I23" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="J23" s="45">
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.2">
@@ -11147,16 +11172,16 @@
         <v>21</v>
       </c>
       <c r="C24" s="38" t="s">
-        <v>124</v>
+        <v>672</v>
       </c>
       <c r="D24" s="43">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E24" s="44" t="s">
-        <v>66</v>
+        <v>673</v>
       </c>
       <c r="F24" s="45">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="G24" s="44" t="s">
         <v>72</v>
@@ -11168,7 +11193,7 @@
         <v>74</v>
       </c>
       <c r="J24" s="45">
-        <v>3</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
@@ -11239,7 +11264,7 @@
         <v>31</v>
       </c>
       <c r="C34" s="38" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D34" s="43">
         <v>12</v>
@@ -11324,7 +11349,7 @@
         <v>40</v>
       </c>
       <c r="C43" s="38" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D43" s="43">
         <v>30</v>
@@ -11429,12 +11454,18 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Effect!$B$6:$B$19</xm:f>
           </x14:formula1>
-          <xm:sqref>I4:I53 E4:E53 G4:G53</xm:sqref>
+          <xm:sqref>I4:I53 G4:G53</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Effect!$B$6:$B$20</xm:f>
+          </x14:formula1>
+          <xm:sqref>E4:E53</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -11447,7 +11478,7 @@
   <dimension ref="B2:AA40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -11490,7 +11521,7 @@
         <v>56</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="G3" s="16" t="s">
         <v>63</v>
@@ -11511,16 +11542,16 @@
         <v>62</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="R3" s="14" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="4" spans="2:25" x14ac:dyDescent="0.2">
@@ -11528,10 +11559,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E4" s="14">
         <v>0</v>
@@ -11540,16 +11571,16 @@
         <v>0</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="O4" s="14" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="R4" s="14" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.2">
@@ -11557,7 +11588,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.2">
@@ -11565,10 +11596,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.2">
@@ -11576,13 +11607,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="M7" s="14" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="O7" s="14" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="8" spans="2:25" x14ac:dyDescent="0.2">
@@ -11590,10 +11621,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="9" spans="2:25" x14ac:dyDescent="0.2">
@@ -11601,16 +11632,16 @@
         <v>6</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="M9" s="14" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="U9" s="14" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="V9" s="37" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.2">
@@ -11618,10 +11649,10 @@
         <v>7</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="M10" s="14" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="11" spans="2:25" x14ac:dyDescent="0.2">
@@ -11629,16 +11660,16 @@
         <v>8</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="M11" s="14" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="U11" s="14" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="V11" s="37" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.2">
@@ -11646,16 +11677,16 @@
         <v>9</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="M12" s="14" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="V12" s="14" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="W12" s="37" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.2">
@@ -11663,19 +11694,19 @@
         <v>10</v>
       </c>
       <c r="C13" s="14" t="s">
+        <v>495</v>
+      </c>
+      <c r="M13" s="14" t="s">
+        <v>600</v>
+      </c>
+      <c r="N13" s="14" t="s">
+        <v>601</v>
+      </c>
+      <c r="V13" s="14" t="s">
         <v>497</v>
       </c>
-      <c r="M13" s="14" t="s">
-        <v>602</v>
-      </c>
-      <c r="N13" s="14" t="s">
-        <v>603</v>
-      </c>
-      <c r="V13" s="14" t="s">
-        <v>499</v>
-      </c>
       <c r="W13" s="37" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.2">
@@ -11683,19 +11714,19 @@
         <v>11</v>
       </c>
       <c r="O14" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="P14" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="Q14" s="14" t="s">
         <v>394</v>
       </c>
-      <c r="P14" s="14" t="s">
-        <v>395</v>
-      </c>
-      <c r="Q14" s="14" t="s">
-        <v>396</v>
-      </c>
       <c r="V14" s="14" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="W14" s="37" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.2">
@@ -11703,10 +11734,10 @@
         <v>12</v>
       </c>
       <c r="V15" s="14" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="W15" s="37" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.2">
@@ -11714,10 +11745,10 @@
         <v>13</v>
       </c>
       <c r="V16" s="14" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="W16" s="37" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="X16" s="37"/>
       <c r="Y16" s="37"/>
@@ -11727,10 +11758,10 @@
         <v>14</v>
       </c>
       <c r="V17" s="14" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="W17" s="37" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="18" spans="2:27" x14ac:dyDescent="0.2">
@@ -11738,10 +11769,10 @@
         <v>15</v>
       </c>
       <c r="V18" s="14" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="W18" s="37" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.2">
@@ -11749,22 +11780,22 @@
         <v>16</v>
       </c>
       <c r="U19" s="14" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="W19" s="14" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="X19" s="14" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="Y19" s="14" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="Z19" s="37" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="AA19" s="14" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.2">
@@ -11772,16 +11803,16 @@
         <v>17</v>
       </c>
       <c r="U20" s="14" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="W20" s="14" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="Y20" s="14" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="Z20" s="37" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.2">
@@ -11789,25 +11820,25 @@
         <v>18</v>
       </c>
       <c r="U21" s="14" t="s">
+        <v>494</v>
+      </c>
+      <c r="V21" s="14" t="s">
         <v>496</v>
       </c>
-      <c r="V21" s="14" t="s">
-        <v>498</v>
-      </c>
       <c r="W21" s="14" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="X21" s="37" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="Y21" s="37" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="Z21" s="37" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="AA21" s="14" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.2">
@@ -11815,45 +11846,57 @@
         <v>19</v>
       </c>
       <c r="V22" s="14" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="W22" s="14" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="X22" s="37" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="Y22" s="37" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="Z22" s="37" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="AA22" s="14" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="23" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B23" s="21">
         <v>20</v>
       </c>
+      <c r="C23" s="14" t="s">
+        <v>669</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>670</v>
+      </c>
+      <c r="E23" s="14">
+        <v>0</v>
+      </c>
+      <c r="F23" s="14">
+        <v>70</v>
+      </c>
       <c r="V23" s="14" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="W23" s="14" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="X23" s="37" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="Y23" s="37" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="Z23" s="37" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="AA23" s="14" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="24" spans="2:27" x14ac:dyDescent="0.2">
@@ -11861,22 +11904,22 @@
         <v>21</v>
       </c>
       <c r="V24" s="14" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="W24" s="14" t="s">
+        <v>513</v>
+      </c>
+      <c r="X24" s="37" t="s">
         <v>515</v>
       </c>
-      <c r="X24" s="37" t="s">
-        <v>517</v>
-      </c>
       <c r="Y24" s="37" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="Z24" s="37" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="AA24" s="14" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="25" spans="2:27" x14ac:dyDescent="0.2">
@@ -11884,19 +11927,19 @@
         <v>22</v>
       </c>
       <c r="V25" s="14" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="W25" s="14" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="X25" s="37" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="Y25" s="37" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="AA25" s="14" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="26" spans="2:27" x14ac:dyDescent="0.2">
@@ -11904,19 +11947,19 @@
         <v>23</v>
       </c>
       <c r="V26" s="14" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="W26" s="14" t="s">
+        <v>529</v>
+      </c>
+      <c r="X26" s="37" t="s">
+        <v>530</v>
+      </c>
+      <c r="Y26" s="37" t="s">
         <v>531</v>
       </c>
-      <c r="X26" s="37" t="s">
-        <v>532</v>
-      </c>
-      <c r="Y26" s="37" t="s">
-        <v>533</v>
-      </c>
       <c r="AA26" s="14" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="27" spans="2:27" x14ac:dyDescent="0.2">
@@ -11924,22 +11967,22 @@
         <v>24</v>
       </c>
       <c r="V27" s="14" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="W27" s="14" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="X27" s="37" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="Y27" s="37" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="Z27" s="37" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="AA27" s="14" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="28" spans="2:27" x14ac:dyDescent="0.2">
@@ -11947,16 +11990,16 @@
         <v>25</v>
       </c>
       <c r="U28" s="14" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="W28" s="14" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="Y28" s="14" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="AA28" s="14" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.2">
@@ -11986,12 +12029,12 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D36" s="14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D40" s="14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -12010,7 +12053,7 @@
   <dimension ref="A2:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -12189,10 +12232,10 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="C18" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -12200,14 +12243,22 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C19" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="15"/>
+      <c r="A20" s="15">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>674</v>
+      </c>
+      <c r="C20" t="s">
+        <v>675</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="15"/>
@@ -12261,8 +12312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T71"/>
   <sheetViews>
-    <sheetView topLeftCell="B37" workbookViewId="0">
-      <selection activeCell="H69" sqref="H69"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -12287,556 +12338,556 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
+        <v>193</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="H4" t="s">
+        <v>309</v>
+      </c>
+      <c r="I4" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="J4" s="25" t="s">
+        <v>308</v>
+      </c>
+      <c r="K4" s="26" t="s">
         <v>195</v>
       </c>
-      <c r="F4" s="25" t="s">
-        <v>196</v>
-      </c>
-      <c r="G4" s="25" t="s">
-        <v>201</v>
-      </c>
-      <c r="H4" t="s">
-        <v>311</v>
-      </c>
-      <c r="I4" s="34" t="s">
-        <v>348</v>
-      </c>
-      <c r="J4" s="25" t="s">
-        <v>310</v>
-      </c>
-      <c r="K4" s="26" t="s">
-        <v>197</v>
-      </c>
       <c r="L4" s="27" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="S4" s="27" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="T4" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="F5" s="26" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G5" s="26" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="L5" s="28" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="N5" s="26" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="O5" s="27" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="S5" s="27" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="T5" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="F6" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="G6" s="27" t="s">
         <v>198</v>
       </c>
-      <c r="G6" s="27" t="s">
-        <v>200</v>
-      </c>
       <c r="H6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="K6" s="26" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="L6" s="27" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="O6" s="27" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="S6" s="27" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="T6" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B7" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>168</v>
-      </c>
       <c r="F7" s="28" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G7" s="28" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H7" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="L7" s="28" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="O7" s="28" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="S7" s="27" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="T7" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K8" s="26" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="L8" s="27" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="M8" s="27" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="S8" s="27" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="T8" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="L9" s="28" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="M9" s="28" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="S9" s="27" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="T9" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F10" t="s">
+        <v>351</v>
+      </c>
+      <c r="G10" t="s">
         <v>353</v>
       </c>
-      <c r="G10" t="s">
-        <v>355</v>
-      </c>
       <c r="K10" s="26" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="L10" s="27" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="S10" s="27" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="T10" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C11" t="s">
+        <v>141</v>
+      </c>
+      <c r="D11" t="s">
         <v>143</v>
       </c>
-      <c r="D11" t="s">
-        <v>145</v>
-      </c>
       <c r="F11" t="s">
+        <v>352</v>
+      </c>
+      <c r="G11" t="s">
         <v>354</v>
       </c>
-      <c r="G11" t="s">
-        <v>356</v>
-      </c>
       <c r="L11" s="25" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="M11" s="26" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="N11" s="27" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="O11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="S11" s="27" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="T11" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="N12" s="26" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="O12" s="27" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="S12" s="27" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="T12" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D13" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="O13" s="28" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="S13" s="27" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="T13" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="O14" s="28" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="N15" s="26" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="O15" s="27" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B16" s="12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
       <c r="O16" s="28" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C17" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H17" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="O17" s="28" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B18" t="s">
+        <v>177</v>
+      </c>
+      <c r="C18" t="s">
+        <v>178</v>
+      </c>
+      <c r="E18" t="s">
         <v>179</v>
       </c>
-      <c r="C18" t="s">
-        <v>180</v>
-      </c>
-      <c r="E18" t="s">
-        <v>181</v>
-      </c>
       <c r="M18" s="26" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="N18" s="27" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="31" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E19" s="67"/>
       <c r="N19" s="28" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="32" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D20" s="32"/>
       <c r="E20" s="67"/>
       <c r="M20" s="26" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="N20" s="27" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D21" s="32"/>
       <c r="E21" s="67"/>
       <c r="N21" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="T21" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="31" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D22" s="31"/>
       <c r="E22" s="67"/>
       <c r="N22" s="25" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="O22" s="26" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="P22" s="27" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="S22" s="28" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="T22" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="31" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B23" s="31" t="s">
+        <v>285</v>
+      </c>
+      <c r="C23" s="31" t="s">
         <v>287</v>
       </c>
-      <c r="C23" s="31" t="s">
-        <v>289</v>
-      </c>
       <c r="D23" s="31" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E23" s="67"/>
       <c r="P23" s="28" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="S23" s="28" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="T23" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B24" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C24" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E24" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="O24" s="28" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="S24" s="28" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="T24" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B25" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E25" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="M25" s="28" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="S25" s="28" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="T25" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K26" s="26" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="L26" s="27" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="S26" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="T26" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C27" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L27" s="28" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="S27" s="28" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="T27" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C28" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K28" s="28" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="S28" s="28" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="T28" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C29" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
@@ -12844,441 +12895,441 @@
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
+        <v>145</v>
+      </c>
+      <c r="C32" t="s">
+        <v>146</v>
+      </c>
+      <c r="D32" t="s">
         <v>147</v>
       </c>
-      <c r="C32" t="s">
-        <v>148</v>
-      </c>
-      <c r="D32" t="s">
-        <v>149</v>
-      </c>
       <c r="I32" s="34" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D33" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C35" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D35" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D36" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D37" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C39" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D39" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
+        <v>184</v>
+      </c>
+      <c r="D40" t="s">
         <v>186</v>
-      </c>
-      <c r="D40" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C41" t="s">
+        <v>185</v>
+      </c>
+      <c r="D41" t="s">
         <v>187</v>
-      </c>
-      <c r="D41" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C42" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D42" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C43" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D43" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C44" t="s">
+        <v>216</v>
+      </c>
+      <c r="D44" t="s">
+        <v>217</v>
+      </c>
+      <c r="H44" t="s">
         <v>218</v>
       </c>
-      <c r="D44" t="s">
-        <v>219</v>
-      </c>
-      <c r="H44" t="s">
-        <v>220</v>
-      </c>
       <c r="I44" t="s">
+        <v>240</v>
+      </c>
+      <c r="J44" t="s">
+        <v>265</v>
+      </c>
+      <c r="K44" t="s">
         <v>242</v>
       </c>
-      <c r="J44" t="s">
-        <v>267</v>
-      </c>
-      <c r="K44" t="s">
-        <v>244</v>
-      </c>
       <c r="L44" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.2">
       <c r="F45" s="29"/>
       <c r="G45" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H45" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="I45" t="s">
+        <v>243</v>
+      </c>
+      <c r="J45" t="s">
+        <v>253</v>
+      </c>
+      <c r="K45" t="s">
         <v>245</v>
       </c>
-      <c r="J45" t="s">
-        <v>255</v>
-      </c>
-      <c r="K45" t="s">
-        <v>247</v>
-      </c>
       <c r="L45" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.2">
       <c r="F46" s="29"/>
       <c r="G46" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H46" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="I46" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="J46" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="K46" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="L46" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F47" s="29"/>
       <c r="G47" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H47" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="I47" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J47" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="K47" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="L47" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F48" s="29"/>
       <c r="G48" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H48" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I48" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J48" t="s">
+        <v>247</v>
+      </c>
+      <c r="K48" t="s">
         <v>249</v>
       </c>
-      <c r="K48" t="s">
-        <v>251</v>
-      </c>
       <c r="L48" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="49" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F49" s="29"/>
       <c r="G49" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H49" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="I49" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J49" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K49" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="L49" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="50" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F50" s="29"/>
       <c r="G50" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H50" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="I50" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="J50" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="K50" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="L50" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="51" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F51" s="29"/>
       <c r="G51" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H51" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="I51" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="J51" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="K51" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="L51" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="52" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F52" s="29"/>
       <c r="G52" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H52" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="I52" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="J52" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="K52" t="s">
+        <v>260</v>
+      </c>
+      <c r="L52" t="s">
         <v>262</v>
-      </c>
-      <c r="L52" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="53" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F53" s="29"/>
       <c r="G53" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H53" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I53" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="J53" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="K53" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L53" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="62" spans="6:14" x14ac:dyDescent="0.2">
       <c r="H62" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J62" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="L62" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="N62" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="63" spans="6:14" ht="57" x14ac:dyDescent="0.2">
       <c r="G63" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H63" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="I63" s="30" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J63" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="L63" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="M63" s="30" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="64" spans="6:14" x14ac:dyDescent="0.2">
       <c r="G64" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H64" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="I64" s="30"/>
       <c r="L64" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="M64" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="65" spans="7:13" x14ac:dyDescent="0.2">
       <c r="G65" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H65" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="I65" s="30"/>
       <c r="L65" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="M65" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="66" spans="7:13" x14ac:dyDescent="0.2">
       <c r="G66" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H66" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="I66" s="30"/>
       <c r="L66" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="M66" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="67" spans="7:13" x14ac:dyDescent="0.2">
       <c r="G67" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H67" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="I67" s="30" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="L67" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="M67" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="68" spans="7:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="G68" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H68" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="I68" s="30" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="L68" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="M68" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="69" spans="7:13" x14ac:dyDescent="0.2">
       <c r="G69" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I69" s="30"/>
       <c r="L69" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="M69" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="70" spans="7:13" x14ac:dyDescent="0.2">
       <c r="G70" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="I70" s="30"/>
     </row>
     <row r="71" spans="7:13" x14ac:dyDescent="0.2">
       <c r="G71" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="I71" s="30"/>
     </row>
@@ -13305,83 +13356,83 @@
   <sheetData>
     <row r="7" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F7" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="8" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="F8" t="s">
+        <v>402</v>
+      </c>
+      <c r="G8" t="s">
         <v>404</v>
-      </c>
-      <c r="G8" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.2">
       <c r="F9" t="s">
+        <v>403</v>
+      </c>
+      <c r="G9" t="s">
         <v>405</v>
-      </c>
-      <c r="G9" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E10" t="s">
+        <v>406</v>
+      </c>
+      <c r="F10" t="s">
+        <v>407</v>
+      </c>
+      <c r="G10" t="s">
         <v>408</v>
-      </c>
-      <c r="F10" t="s">
-        <v>409</v>
-      </c>
-      <c r="G10" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="15" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="16" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D17" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="18" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D18" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="19" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D19" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="20" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D20" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="21" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D21" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
   </sheetData>

</xml_diff>